<commit_message>
Update with latest merged data.
</commit_message>
<xml_diff>
--- a/merged_sim_data.xlsx
+++ b/merged_sim_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbaker\source\repos\puzzle_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CC2E7D-DA89-471B-9416-764BB293B7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361E6E66-49BB-4B92-8E11-936CE1F509E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4950" yWindow="4460" windowWidth="28800" windowHeight="15370" xr2:uid="{28FD9770-0A94-4093-8D11-2FB132A28C6B}"/>
   </bookViews>
@@ -228,10 +228,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$274</c:f>
+              <c:f>Sheet1!$B$2:$B$299</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="273"/>
+                <c:ptCount val="298"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -1050,16 +1050,91 @@
                 </c:pt>
                 <c:pt idx="272">
                   <c:v>75625</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>76176</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>76729</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>77284</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>77841</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>78400</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>78961</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>79524</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>80089</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>80656</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>81225</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>81796</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>82369</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>82944</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>83521</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>84100</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>84681</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>85849</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>86436</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>87025</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>87616</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>88209</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>88804</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>89401</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>90000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$274</c:f>
+              <c:f>Sheet1!$D$2:$D$299</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="273"/>
+                <c:ptCount val="298"/>
                 <c:pt idx="0">
                   <c:v>1.1121137599944584</c:v>
                 </c:pt>
@@ -1878,6 +1953,81 @@
                 </c:pt>
                 <c:pt idx="272">
                   <c:v>1.3898284444739142</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1.3846918138848627</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1.3821378592988671</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1.3826183151399687</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>1.386109763728693</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>1.3983388871414875</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>1.3891891718021849</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>1.3832783032911289</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>1.3817961161936241</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>1.3850082917101112</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>1.396896015759721</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>1.3868722310655341</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>1.3819137627631131</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>1.3828753358796071</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>1.3991834984756504</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>1.3871067319681714</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>1.381829983193821</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>1.3840486420056375</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>1.3947904147838417</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>1.384112394635721</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>1.3816193419882867</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>1.4000755827962099</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>1.3863106137281505</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>1.3814397843071982</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>1.4015900120530753</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>1.3868012046807607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1885,7 +2035,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C599-42E9-8181-812EF603A9DD}"/>
+              <c16:uniqueId val="{00000000-9D56-4BC5-B51A-13A7153D964A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1897,11 +2047,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="135490800"/>
-        <c:axId val="135479280"/>
+        <c:axId val="746417151"/>
+        <c:axId val="746418111"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135490800"/>
+        <c:axId val="746417151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,12 +2108,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135479280"/>
+        <c:crossAx val="746418111"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135479280"/>
+        <c:axId val="746418111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2020,7 +2170,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135490800"/>
+        <c:crossAx val="746417151"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2630,22 +2780,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:colOff>333374</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACEE85AD-7324-D175-962B-67593A5BA4D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC1EBE2C-FCAC-05FC-9D4B-AB3CDC4413D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2983,16 +3133,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000BE2E6-D01C-47B4-BE7D-344FFD3EC8EB}">
-  <dimension ref="A1:D274"/>
+  <dimension ref="A1:D299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D274"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -6875,7 +7026,7 @@
         <v>6352385.625</v>
       </c>
       <c r="D259">
-        <f t="shared" ref="D259:D274" si="4">LOG(C259,B259)</f>
+        <f t="shared" ref="D259:D299" si="4">LOG(C259,B259)</f>
         <v>1.4084910833522306</v>
       </c>
     </row>
@@ -7102,6 +7253,381 @@
       <c r="D274">
         <f t="shared" si="4"/>
         <v>1.3898284444739142</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A275">
+        <v>16000</v>
+      </c>
+      <c r="B275">
+        <v>76176</v>
+      </c>
+      <c r="C275">
+        <v>5751930.75</v>
+      </c>
+      <c r="D275">
+        <f t="shared" si="4"/>
+        <v>1.3846918138848627</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A276">
+        <v>16000</v>
+      </c>
+      <c r="B276">
+        <v>76729</v>
+      </c>
+      <c r="C276">
+        <v>5645306.40625</v>
+      </c>
+      <c r="D276">
+        <f t="shared" si="4"/>
+        <v>1.3821378592988671</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A277">
+        <v>16000</v>
+      </c>
+      <c r="B277">
+        <v>77284</v>
+      </c>
+      <c r="C277">
+        <v>5732739.34375</v>
+      </c>
+      <c r="D277">
+        <f t="shared" si="4"/>
+        <v>1.3826183151399687</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A278">
+        <v>16000</v>
+      </c>
+      <c r="B278">
+        <v>77841</v>
+      </c>
+      <c r="C278">
+        <v>6022152.21875</v>
+      </c>
+      <c r="D278">
+        <f t="shared" si="4"/>
+        <v>1.386109763728693</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A279">
+        <v>16000</v>
+      </c>
+      <c r="B279">
+        <v>78400</v>
+      </c>
+      <c r="C279">
+        <v>6980917.03125</v>
+      </c>
+      <c r="D279">
+        <f t="shared" si="4"/>
+        <v>1.3983388871414875</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A280">
+        <v>16000</v>
+      </c>
+      <c r="B280">
+        <v>78961</v>
+      </c>
+      <c r="C280">
+        <v>6359641.125</v>
+      </c>
+      <c r="D280">
+        <f t="shared" si="4"/>
+        <v>1.3891891718021849</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A281">
+        <v>16000</v>
+      </c>
+      <c r="B281">
+        <v>79524</v>
+      </c>
+      <c r="C281">
+        <v>6008317.28125</v>
+      </c>
+      <c r="D281">
+        <f t="shared" si="4"/>
+        <v>1.3832783032911289</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A282">
+        <v>16000</v>
+      </c>
+      <c r="B282">
+        <v>80089</v>
+      </c>
+      <c r="C282">
+        <v>5966751.46875</v>
+      </c>
+      <c r="D282">
+        <f t="shared" si="4"/>
+        <v>1.3817961161936241</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A283">
+        <v>16000</v>
+      </c>
+      <c r="B283">
+        <v>80656</v>
+      </c>
+      <c r="C283">
+        <v>6247877.21875</v>
+      </c>
+      <c r="D283">
+        <f t="shared" si="4"/>
+        <v>1.3850082917101112</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A284">
+        <v>16000</v>
+      </c>
+      <c r="B284">
+        <v>81225</v>
+      </c>
+      <c r="C284">
+        <v>7216489.90625</v>
+      </c>
+      <c r="D284">
+        <f t="shared" si="4"/>
+        <v>1.396896015759721</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A285">
+        <v>16000</v>
+      </c>
+      <c r="B285">
+        <v>81796</v>
+      </c>
+      <c r="C285">
+        <v>6506264</v>
+      </c>
+      <c r="D285">
+        <f t="shared" si="4"/>
+        <v>1.3868722310655341</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A286">
+        <v>16000</v>
+      </c>
+      <c r="B286">
+        <v>82369</v>
+      </c>
+      <c r="C286">
+        <v>6211001.59375</v>
+      </c>
+      <c r="D286">
+        <f t="shared" si="4"/>
+        <v>1.3819137627631131</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A287">
+        <v>16000</v>
+      </c>
+      <c r="B287">
+        <v>82944</v>
+      </c>
+      <c r="C287">
+        <v>6339666.6875</v>
+      </c>
+      <c r="D287">
+        <f t="shared" si="4"/>
+        <v>1.3828753358796071</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A288">
+        <v>16000</v>
+      </c>
+      <c r="B288">
+        <v>83521</v>
+      </c>
+      <c r="C288">
+        <v>7700081.21875</v>
+      </c>
+      <c r="D288">
+        <f t="shared" si="4"/>
+        <v>1.3991834984756504</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A289">
+        <v>16000</v>
+      </c>
+      <c r="B289">
+        <v>84100</v>
+      </c>
+      <c r="C289">
+        <v>6779812.4375</v>
+      </c>
+      <c r="D289">
+        <f t="shared" si="4"/>
+        <v>1.3871067319681714</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A290">
+        <v>16000</v>
+      </c>
+      <c r="B290">
+        <v>84681</v>
+      </c>
+      <c r="C290">
+        <v>6447070.4375</v>
+      </c>
+      <c r="D290">
+        <f t="shared" si="4"/>
+        <v>1.381829983193821</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A291">
+        <v>16000</v>
+      </c>
+      <c r="B291">
+        <v>85264</v>
+      </c>
+      <c r="C291">
+        <v>6674512.875</v>
+      </c>
+      <c r="D291">
+        <f t="shared" si="4"/>
+        <v>1.3840486420056375</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A292">
+        <v>16000</v>
+      </c>
+      <c r="B292">
+        <v>85849</v>
+      </c>
+      <c r="C292">
+        <v>7612488.03125</v>
+      </c>
+      <c r="D292">
+        <f t="shared" si="4"/>
+        <v>1.3947904147838417</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A293">
+        <v>16000</v>
+      </c>
+      <c r="B293">
+        <v>86436</v>
+      </c>
+      <c r="C293">
+        <v>6806757.34375</v>
+      </c>
+      <c r="D293">
+        <f t="shared" si="4"/>
+        <v>1.384112394635721</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A294">
+        <v>16000</v>
+      </c>
+      <c r="B294">
+        <v>87025</v>
+      </c>
+      <c r="C294">
+        <v>6678943</v>
+      </c>
+      <c r="D294">
+        <f t="shared" si="4"/>
+        <v>1.3816193419882867</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A295">
+        <v>16000</v>
+      </c>
+      <c r="B295">
+        <v>87616</v>
+      </c>
+      <c r="C295">
+        <v>8317453.1875</v>
+      </c>
+      <c r="D295">
+        <f t="shared" si="4"/>
+        <v>1.4000755827962099</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A296">
+        <v>16000</v>
+      </c>
+      <c r="B296">
+        <v>88209</v>
+      </c>
+      <c r="C296">
+        <v>7178224.25</v>
+      </c>
+      <c r="D296">
+        <f t="shared" si="4"/>
+        <v>1.3863106137281505</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A297">
+        <v>16000</v>
+      </c>
+      <c r="B297">
+        <v>88804</v>
+      </c>
+      <c r="C297">
+        <v>6854275.625</v>
+      </c>
+      <c r="D297">
+        <f t="shared" si="4"/>
+        <v>1.3814397843071982</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A298">
+        <v>16000</v>
+      </c>
+      <c r="B298">
+        <v>89401</v>
+      </c>
+      <c r="C298">
+        <v>8704664.1875</v>
+      </c>
+      <c r="D298">
+        <f t="shared" si="4"/>
+        <v>1.4015900120530753</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A299">
+        <v>16000</v>
+      </c>
+      <c r="B299">
+        <v>90000</v>
+      </c>
+      <c r="C299">
+        <v>7422487.59375</v>
+      </c>
+      <c r="D299">
+        <f t="shared" si="4"/>
+        <v>1.3868012046807607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>